<commit_message>
Atualização de dados e mais UDF's
</commit_message>
<xml_diff>
--- a/Projeto/dados.xlsx
+++ b/Projeto/dados.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hacker/Desktop/UA/BD/bd/Projeto/working/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paiva/Documents/Universidade/Engenharia Informática/2º Ano/2º Semestre/Base de Dados/bd/Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA8D81D-1B97-1647-82CA-4F3BF9F7F869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9A76F7-AA08-0A46-995B-52FD27E309E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" firstSheet="2" activeTab="6" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" firstSheet="4" activeTab="5" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cupao" sheetId="3" r:id="rId1"/>
-    <sheet name="ClienteUsaCupão" sheetId="14" r:id="rId2"/>
-    <sheet name="ClienteFavorita" sheetId="15" r:id="rId3"/>
-    <sheet name="Promoção" sheetId="4" r:id="rId4"/>
-    <sheet name="ProdutoTemPromoção" sheetId="16" r:id="rId5"/>
-    <sheet name="Produto" sheetId="2" r:id="rId6"/>
-    <sheet name="Contacto" sheetId="7" r:id="rId7"/>
-    <sheet name="Cosmética" sheetId="5" r:id="rId8"/>
-    <sheet name="Perfume" sheetId="6" r:id="rId9"/>
-    <sheet name="Compra" sheetId="8" r:id="rId10"/>
-    <sheet name="Presencial" sheetId="19" r:id="rId11"/>
-    <sheet name="Online" sheetId="20" r:id="rId12"/>
-    <sheet name="CompraTemProduto" sheetId="17" r:id="rId13"/>
-    <sheet name="Utilizador" sheetId="9" r:id="rId14"/>
-    <sheet name="Cliente" sheetId="10" r:id="rId15"/>
-    <sheet name="Funcionário" sheetId="11" r:id="rId16"/>
-    <sheet name="Serviço" sheetId="12" r:id="rId17"/>
-    <sheet name="FuncFazServiço" sheetId="18" r:id="rId18"/>
+    <sheet name="cupao" sheetId="3" r:id="rId1"/>
+    <sheet name="cliente_usa_cupao" sheetId="14" r:id="rId2"/>
+    <sheet name="clientefavorita" sheetId="15" r:id="rId3"/>
+    <sheet name="promocao" sheetId="4" r:id="rId4"/>
+    <sheet name="produto_tem_promocao" sheetId="16" r:id="rId5"/>
+    <sheet name="produto" sheetId="2" r:id="rId6"/>
+    <sheet name="contacto" sheetId="7" r:id="rId7"/>
+    <sheet name="cosmetica" sheetId="5" r:id="rId8"/>
+    <sheet name="perfume" sheetId="6" r:id="rId9"/>
+    <sheet name="compra" sheetId="8" r:id="rId10"/>
+    <sheet name="compra_presencial" sheetId="19" r:id="rId11"/>
+    <sheet name="compra_online" sheetId="20" r:id="rId12"/>
+    <sheet name="compra_tem_produto" sheetId="17" r:id="rId13"/>
+    <sheet name="utilizador" sheetId="9" r:id="rId14"/>
+    <sheet name="cliente" sheetId="10" r:id="rId15"/>
+    <sheet name="funcionario" sheetId="11" r:id="rId16"/>
+    <sheet name="servico" sheetId="12" r:id="rId17"/>
+    <sheet name="funcionario_faz_servico" sheetId="18" r:id="rId18"/>
     <sheet name="Marcação" sheetId="13" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="413">
   <si>
     <t>id</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Azzaro</t>
   </si>
   <si>
-    <t>preço</t>
-  </si>
-  <si>
     <t>familiaolfativa</t>
   </si>
   <si>
@@ -494,27 +491,15 @@
     <t>Mãos e Pés</t>
   </si>
   <si>
-    <t>utilizadoremail</t>
-  </si>
-  <si>
     <t>telemovel</t>
   </si>
   <si>
     <t>visibilidade</t>
   </si>
   <si>
-    <t>codigoposta</t>
-  </si>
-  <si>
-    <t>país</t>
-  </si>
-  <si>
     <t>endereco</t>
   </si>
   <si>
-    <t>ap/suite/andar</t>
-  </si>
-  <si>
     <t>localidade</t>
   </si>
   <si>
@@ -1151,9 +1136,6 @@
     <t>Mb Way</t>
   </si>
   <si>
-    <t>administrador</t>
-  </si>
-  <si>
     <t>salario</t>
   </si>
   <si>
@@ -1229,9 +1211,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>cupaoid</t>
-  </si>
-  <si>
     <t>2020-02-24 06:30:50.000</t>
   </si>
   <si>
@@ -1244,42 +1223,15 @@
     <t>1U37L2GRMQ</t>
   </si>
   <si>
-    <t>produtoID</t>
-  </si>
-  <si>
-    <t>PromocaoID</t>
-  </si>
-  <si>
-    <t>numerocompra</t>
-  </si>
-  <si>
-    <t>ProdutoID</t>
-  </si>
-  <si>
-    <t>Unidades</t>
-  </si>
-  <si>
-    <t>duracaoMedia</t>
-  </si>
-  <si>
-    <t>funcEmail</t>
-  </si>
-  <si>
     <t>rating</t>
   </si>
   <si>
-    <t>observaçoes</t>
-  </si>
-  <si>
     <t>rastreamento</t>
   </si>
   <si>
     <t>presente</t>
   </si>
   <si>
-    <t>contactoID</t>
-  </si>
-  <si>
     <t>Muito bom produto!</t>
   </si>
   <si>
@@ -1296,6 +1248,48 @@
   </si>
   <si>
     <t>pbFcSarhTbZqz5wTk7mk</t>
+  </si>
+  <si>
+    <t>cupao_id</t>
+  </si>
+  <si>
+    <t>produtoid</t>
+  </si>
+  <si>
+    <t>promocaoid</t>
+  </si>
+  <si>
+    <t>utilizador_email</t>
+  </si>
+  <si>
+    <t>codigo_postal</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>apartamento</t>
+  </si>
+  <si>
+    <t>funcemail</t>
+  </si>
+  <si>
+    <t>observação</t>
+  </si>
+  <si>
+    <t>contactoid</t>
+  </si>
+  <si>
+    <t>compranumero</t>
+  </si>
+  <si>
+    <t>unidades</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>duracao_media</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1388,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1411,7 +1405,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1709,9 +1703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECE3593-E1CC-8E4B-A47B-B25F5CCC3F7D}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -1863,10 +1855,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -1877,10 +1869,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="B12" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1899,7 +1891,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1914,25 +1906,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" t="s">
         <v>228</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>229</v>
-      </c>
-      <c r="C1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1946,7 +1938,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1963,10 +1955,10 @@
         <v>37121343</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1983,10 +1975,10 @@
         <v>60474094</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -2003,10 +1995,10 @@
         <v>86134119</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2023,10 +2015,10 @@
         <v>6421976</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2043,10 +2035,10 @@
         <v>299678786</v>
       </c>
       <c r="C7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2063,10 +2055,10 @@
         <v>111498402</v>
       </c>
       <c r="C8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2083,10 +2075,10 @@
         <v>108025260</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -2103,10 +2095,10 @@
         <v>141414204</v>
       </c>
       <c r="C10" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2123,10 +2115,10 @@
         <v>56737679</v>
       </c>
       <c r="C11" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -2143,10 +2135,10 @@
         <v>3544357</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2163,10 +2155,10 @@
         <v>196674321</v>
       </c>
       <c r="C13" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2183,10 +2175,10 @@
         <v>196954062</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D14" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2203,10 +2195,10 @@
         <v>42896574</v>
       </c>
       <c r="C15" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F15">
         <v>20</v>
@@ -2223,10 +2215,10 @@
         <v>112964237</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -2246,7 +2238,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2256,10 +2248,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2267,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2275,7 +2267,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2283,7 +2275,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2291,7 +2283,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2299,7 +2291,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2307,7 +2299,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -2328,7 +2320,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2340,19 +2332,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D1" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="E1" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="F1" t="s">
         <v>408</v>
@@ -2366,7 +2358,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2394,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2411,7 +2403,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2428,7 +2420,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2467,10 +2459,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2500,7 +2492,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2510,13 +2502,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="B1" t="s">
         <v>400</v>
       </c>
       <c r="C1" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2749,7 +2741,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2765,48 +2757,48 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B2" s="3">
         <v>287567665</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -2815,7 +2807,7 @@
         <v>31905</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I2" s="3">
         <v>2</v>
@@ -2823,19 +2815,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3">
         <v>457253189</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -2844,27 +2836,27 @@
         <v>34368</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B4" s="3">
         <v>998232166</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -2873,27 +2865,27 @@
         <v>37279</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B5" s="3">
         <v>397543100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2902,7 +2894,7 @@
         <v>36135</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
@@ -2910,19 +2902,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B6" s="3">
         <v>302167890</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -2931,27 +2923,27 @@
         <v>22224</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B7" s="3">
         <v>592165320</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -2960,27 +2952,27 @@
         <v>34956</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B8" s="3">
         <v>943212111</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -2989,7 +2981,7 @@
         <v>36292</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I8" s="3">
         <v>14</v>
@@ -2997,19 +2989,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B9" s="3">
         <v>123222985</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -3018,27 +3010,27 @@
         <v>38708</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B10" s="3">
         <v>445976504</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -3047,27 +3039,27 @@
         <v>33061</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B11" s="3">
         <v>455129988</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -3076,7 +3068,7 @@
         <v>36651</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I11" s="3">
         <v>4</v>
@@ -3084,19 +3076,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B12" s="3">
         <v>178495829</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -3105,27 +3097,27 @@
         <v>38266</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B13" s="3">
         <v>125873530</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -3134,7 +3126,7 @@
         <v>26474</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I13" s="3">
         <v>8</v>
@@ -3142,19 +3134,19 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B14" s="3">
         <v>573975939</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F14" s="3">
         <v>0</v>
@@ -3163,27 +3155,27 @@
         <v>36199</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B15" s="3">
         <v>258759872</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -3192,7 +3184,7 @@
         <v>31077</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I15" s="3">
         <v>9</v>
@@ -3200,19 +3192,19 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B16" s="3">
         <v>287352385</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
@@ -3221,7 +3213,7 @@
         <v>36647</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I16" s="3">
         <v>10</v>
@@ -3229,19 +3221,19 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="7" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B17" s="3">
         <v>821358756</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -3250,27 +3242,27 @@
         <v>32766</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B18" s="3">
         <v>602941753</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -3279,7 +3271,7 @@
         <v>37289</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I18" s="3">
         <v>11</v>
@@ -3287,19 +3279,19 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B19" s="3">
         <v>219589974</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -3308,27 +3300,27 @@
         <v>24101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B20" s="3">
         <v>476638927</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
@@ -3337,27 +3329,27 @@
         <v>35868</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B21" s="3">
         <v>593967351</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -3366,7 +3358,7 @@
         <v>29006</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I21" s="3">
         <v>12</v>
@@ -3374,19 +3366,19 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B22" s="3">
         <v>129885782</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
@@ -3395,10 +3387,10 @@
         <v>25857</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3554,21 +3546,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B2" s="3">
         <v>50</v>
@@ -3577,12 +3569,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -3591,12 +3583,12 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B4" s="3">
         <v>100</v>
@@ -3605,12 +3597,12 @@
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B5" s="3">
         <v>100</v>
@@ -3619,12 +3611,12 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -3633,12 +3625,12 @@
         <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B7" s="3">
         <v>200</v>
@@ -3647,12 +3639,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B8" s="3">
         <v>150</v>
@@ -3661,12 +3653,12 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B9" s="3">
         <v>50</v>
@@ -3675,12 +3667,12 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B10" s="3">
         <v>100</v>
@@ -3689,12 +3681,12 @@
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -3703,12 +3695,12 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B12" s="3">
         <v>250</v>
@@ -3717,12 +3709,12 @@
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -3731,12 +3723,12 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -3745,12 +3737,12 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B15" s="3">
         <v>50</v>
@@ -3759,12 +3751,12 @@
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B16" s="3">
         <v>100</v>
@@ -3773,12 +3765,12 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -3787,12 +3779,12 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -3801,7 +3793,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3833,7 +3825,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3845,18 +3837,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>411</v>
       </c>
       <c r="C1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3867,7 +3859,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -3878,7 +3870,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3889,7 +3881,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3914,7 +3906,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3927,10 +3919,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3938,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C2">
         <v>45.5</v>
@@ -3949,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C3">
         <v>7.5</v>
@@ -3960,7 +3952,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C4">
         <v>12.8</v>
@@ -3971,7 +3963,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C5">
         <v>9.5</v>
@@ -3982,7 +3974,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -3993,7 +3985,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -4004,7 +3996,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C8">
         <v>85</v>
@@ -4015,7 +4007,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C9">
         <v>35.700000000000003</v>
@@ -4026,7 +4018,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C10">
         <v>24.5</v>
@@ -4037,7 +4029,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C11">
         <v>47</v>
@@ -4048,7 +4040,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C12">
         <v>14.99</v>
@@ -4059,7 +4051,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C13">
         <v>17.899999999999999</v>
@@ -4070,7 +4062,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -4081,7 +4073,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C15">
         <v>19.989999999999998</v>
@@ -4092,7 +4084,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C16">
         <v>25.15</v>
@@ -4103,7 +4095,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C17">
         <v>23</v>
@@ -4114,7 +4106,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C18">
         <v>67.900000000000006</v>
@@ -4125,7 +4117,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C19">
         <v>20.149999999999999</v>
@@ -4136,7 +4128,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C20">
         <v>71</v>
@@ -4152,7 +4144,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4163,18 +4155,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>384</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="C1" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4185,7 +4177,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -4196,7 +4188,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -4207,7 +4199,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -4218,7 +4210,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -4229,7 +4221,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -4240,7 +4232,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -4251,7 +4243,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B9">
         <v>19</v>
@@ -4262,7 +4254,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4273,7 +4265,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -4284,7 +4276,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -4295,7 +4287,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -4306,7 +4298,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -4317,7 +4309,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -4328,7 +4320,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -4339,7 +4331,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B17">
         <v>13</v>
@@ -4350,7 +4342,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -4361,7 +4353,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4372,7 +4364,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4383,7 +4375,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B21">
         <v>14</v>
@@ -4394,7 +4386,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B22">
         <v>16</v>
@@ -4405,7 +4397,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B23">
         <v>17</v>
@@ -4416,7 +4408,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B24">
         <v>18</v>
@@ -4427,7 +4419,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -4438,7 +4430,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4449,7 +4441,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -4460,7 +4452,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -4471,7 +4463,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -4482,7 +4474,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -4493,7 +4485,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -4504,7 +4496,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B32">
         <v>7</v>
@@ -4515,7 +4507,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -4526,7 +4518,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B34">
         <v>9</v>
@@ -4537,7 +4529,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B35">
         <v>10</v>
@@ -4548,7 +4540,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B36">
         <v>11</v>
@@ -4559,7 +4551,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B37">
         <v>12</v>
@@ -4570,7 +4562,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B38">
         <v>13</v>
@@ -4581,7 +4573,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B39">
         <v>14</v>
@@ -4592,7 +4584,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B40">
         <v>15</v>
@@ -4603,7 +4595,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B41">
         <v>16</v>
@@ -4614,7 +4606,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B42">
         <v>17</v>
@@ -4625,7 +4617,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B43">
         <v>18</v>
@@ -4636,7 +4628,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B44">
         <v>19</v>
@@ -4689,16 +4681,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4706,13 +4698,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E2" s="10">
         <v>43966.6875</v>
@@ -4723,13 +4715,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C3" s="1">
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E3" s="10">
         <v>43996.395833333336</v>
@@ -4740,13 +4732,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C4" s="1">
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E4" s="10">
         <v>43962.791666666664</v>
@@ -4757,13 +4749,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E5" s="10">
         <v>43985.625</v>
@@ -4774,13 +4766,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C6" s="1">
         <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E6" s="10">
         <v>44014.479166666664</v>
@@ -4791,13 +4783,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E7" s="10">
         <v>43966.729166666664</v>
@@ -4808,13 +4800,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C8" s="1">
         <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E8" s="10">
         <v>43974.59375</v>
@@ -4846,7 +4838,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4858,39 +4850,39 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -4898,39 +4890,39 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B6" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B8" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B9" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -4938,26 +4930,26 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B11" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B12" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B13" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -4983,7 +4975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89BB075-E1D3-504E-AEC5-3A48EA5B9950}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4993,15 +4987,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
@@ -5009,7 +5003,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -5017,7 +5011,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B4" s="1">
         <v>6</v>
@@ -5025,7 +5019,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
@@ -5033,7 +5027,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -5041,7 +5035,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B7">
         <v>13</v>
@@ -5049,7 +5043,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -5057,7 +5051,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -5065,7 +5059,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -5073,7 +5067,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -5081,7 +5075,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -5089,7 +5083,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -5097,7 +5091,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B14">
         <v>16</v>
@@ -5105,7 +5099,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -5113,7 +5107,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B16">
         <v>20</v>
@@ -5354,7 +5348,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5365,10 +5359,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5484,8 +5478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6798383C-D243-9640-A634-7870B6E05811}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5508,37 +5502,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
       </c>
       <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>66</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>67</v>
-      </c>
-      <c r="L1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -5549,34 +5543,34 @@
         <v>75.25</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5587,34 +5581,34 @@
         <v>71.3</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5625,34 +5619,34 @@
         <v>81.650000000000006</v>
       </c>
       <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
         <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
       </c>
       <c r="H4">
         <v>100</v>
       </c>
       <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -5663,31 +5657,31 @@
         <v>27.2</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5">
         <v>150</v>
       </c>
       <c r="I5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="K5">
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5698,31 +5692,31 @@
         <v>77.3</v>
       </c>
       <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
       </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
       <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s">
         <v>85</v>
-      </c>
-      <c r="F6" t="s">
-        <v>86</v>
       </c>
       <c r="H6">
         <v>50</v>
       </c>
       <c r="I6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="K6">
         <v>10</v>
       </c>
       <c r="L6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5733,31 +5727,31 @@
         <v>75.25</v>
       </c>
       <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
         <v>90</v>
       </c>
-      <c r="E7" t="s">
-        <v>91</v>
-      </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="K7">
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5768,34 +5762,34 @@
         <v>78.709999999999994</v>
       </c>
       <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>98</v>
       </c>
-      <c r="F8" t="s">
-        <v>99</v>
-      </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8">
         <v>50</v>
       </c>
       <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="K8">
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5806,34 +5800,34 @@
         <v>104.95</v>
       </c>
       <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
         <v>97</v>
       </c>
-      <c r="D9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>98</v>
       </c>
-      <c r="F9" t="s">
-        <v>99</v>
-      </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="K9">
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5844,34 +5838,34 @@
         <v>140.65</v>
       </c>
       <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
         <v>97</v>
       </c>
-      <c r="D10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>98</v>
       </c>
-      <c r="F10" t="s">
-        <v>99</v>
-      </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H10">
         <v>200</v>
       </c>
       <c r="I10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="K10">
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5882,34 +5876,34 @@
         <v>27.3</v>
       </c>
       <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
         <v>97</v>
       </c>
-      <c r="D11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>98</v>
       </c>
-      <c r="F11" t="s">
-        <v>99</v>
-      </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11">
         <v>75</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K11">
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -5920,34 +5914,34 @@
         <v>27.3</v>
       </c>
       <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="D12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>98</v>
       </c>
-      <c r="F12" t="s">
-        <v>99</v>
-      </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H12">
         <v>150</v>
       </c>
       <c r="I12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K12">
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5958,28 +5952,28 @@
         <v>72.5</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13">
         <v>50</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K13">
         <v>2</v>
       </c>
       <c r="L13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -5990,28 +5984,28 @@
         <v>47.5</v>
       </c>
       <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
         <v>108</v>
       </c>
-      <c r="E14" t="s">
-        <v>109</v>
-      </c>
       <c r="F14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H14">
         <v>200</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K14">
         <v>5</v>
       </c>
       <c r="L14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -6022,25 +6016,25 @@
         <v>77.900000000000006</v>
       </c>
       <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="K15">
         <v>5</v>
       </c>
       <c r="L15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -6051,28 +6045,28 @@
         <v>22.28</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" t="s">
         <v>113</v>
-      </c>
-      <c r="G16" t="s">
-        <v>114</v>
       </c>
       <c r="H16">
         <v>30</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K16">
         <v>2</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -6083,28 +6077,28 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" t="s">
         <v>113</v>
-      </c>
-      <c r="G17" t="s">
-        <v>114</v>
       </c>
       <c r="H17">
         <v>50</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K17">
         <v>3</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -6115,28 +6109,28 @@
         <v>50.2</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" t="s">
         <v>113</v>
-      </c>
-      <c r="G18" t="s">
-        <v>114</v>
       </c>
       <c r="H18">
         <v>100</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K18">
         <v>4</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -6147,28 +6141,28 @@
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
         <v>113</v>
-      </c>
-      <c r="G19" t="s">
-        <v>114</v>
       </c>
       <c r="H19">
         <v>75</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K19">
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6179,25 +6173,25 @@
         <v>29.7</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20">
         <v>30</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6208,25 +6202,25 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21">
         <v>50</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K21">
         <v>6</v>
       </c>
       <c r="L21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -6237,28 +6231,28 @@
         <v>47.45</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H22">
         <v>100</v>
       </c>
       <c r="I22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -6269,31 +6263,31 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H23">
         <v>100</v>
       </c>
       <c r="I23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="K23">
         <v>5</v>
       </c>
       <c r="L23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -6304,19 +6298,19 @@
         <v>38.65</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H24">
         <v>125</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K24">
         <v>6</v>
@@ -6330,22 +6324,22 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H25">
         <v>200</v>
       </c>
       <c r="I25" t="s">
+        <v>137</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -6359,19 +6353,19 @@
         <v>32.950000000000003</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H26">
         <v>100</v>
       </c>
       <c r="J26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K26">
         <v>3</v>
@@ -6412,8 +6406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9452136D-12A1-A84C-959A-D16ED4D29668}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6433,28 +6427,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
         <v>147</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G1" t="s">
         <v>148</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>405</v>
+      </c>
+      <c r="I1" t="s">
         <v>149</v>
-      </c>
-      <c r="E1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6462,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C2">
         <v>914363252</v>
@@ -6471,16 +6465,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -6488,7 +6482,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C3">
         <v>924763965</v>
@@ -6497,19 +6491,19 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" t="s">
         <v>156</v>
       </c>
-      <c r="G3" t="s">
-        <v>161</v>
-      </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -6517,7 +6511,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C4">
         <v>914274915</v>
@@ -6526,19 +6520,19 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -6546,7 +6540,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C5">
         <v>964829602</v>
@@ -6555,19 +6549,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -6575,7 +6569,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C6">
         <v>935502152</v>
@@ -6584,19 +6578,19 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -6604,7 +6598,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C7">
         <v>914628560</v>
@@ -6613,19 +6607,19 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G7" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6633,7 +6627,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C8">
         <v>963926453</v>
@@ -6642,19 +6636,19 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -6662,7 +6656,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C9">
         <v>921547935</v>
@@ -6671,19 +6665,19 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -6691,7 +6685,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C10">
         <v>918426539</v>
@@ -6700,19 +6694,19 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H10" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I10" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -6720,7 +6714,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C11">
         <v>963159731</v>
@@ -6729,19 +6723,19 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I11" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -6749,7 +6743,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C12">
         <v>936267422</v>
@@ -6758,16 +6752,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I12" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -6775,7 +6769,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C13">
         <v>926375015</v>
@@ -6784,19 +6778,19 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G13" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H13" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -6804,7 +6798,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C14">
         <v>963216832</v>
@@ -6813,19 +6807,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G14" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H14" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -6833,7 +6827,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C15">
         <v>915392054</v>
@@ -6842,16 +6836,16 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G15" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -6859,7 +6853,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C16">
         <v>964667921</v>
@@ -6868,19 +6862,19 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G16" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I16" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -6888,7 +6882,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C17">
         <v>962468333</v>
@@ -6897,19 +6891,19 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F17" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G17" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I17" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -6917,7 +6911,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C18">
         <v>925488312</v>
@@ -6926,19 +6920,19 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I18" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -6946,7 +6940,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C19">
         <v>915424675</v>
@@ -6955,16 +6949,16 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G19" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -6972,7 +6966,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C20">
         <v>963215352</v>
@@ -6981,19 +6975,19 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G20" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -7001,7 +6995,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C21">
         <v>924583100</v>
@@ -7010,16 +7004,16 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G21" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I21" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -7064,7 +7058,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7072,7 +7066,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7080,7 +7074,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7088,7 +7082,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuação alteração dos dados, script python para inserção e SQL Programming
Co-authored-by: pedro.bas@ua.pt <pedro.bas@ua.pt>
</commit_message>
<xml_diff>
--- a/Projeto/dados.xlsx
+++ b/Projeto/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paiva/Documents/Universidade/Engenharia Informática/2º Ano/2º Semestre/Base de Dados/bd/Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9A76F7-AA08-0A46-995B-52FD27E309E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD042977-B6DD-2E42-AE9C-16BDC06E3EEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" firstSheet="4" activeTab="5" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" firstSheet="5" activeTab="18" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
   </bookViews>
   <sheets>
     <sheet name="cupao" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="funcionario" sheetId="11" r:id="rId16"/>
     <sheet name="servico" sheetId="12" r:id="rId17"/>
     <sheet name="funcionario_faz_servico" sheetId="18" r:id="rId18"/>
-    <sheet name="Marcação" sheetId="13" r:id="rId19"/>
+    <sheet name="marcacao" sheetId="13" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1208,9 +1208,6 @@
     <t>funcionario_email</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>2020-02-24 06:30:50.000</t>
   </si>
   <si>
@@ -1290,6 +1287,9 @@
   </si>
   <si>
     <t>duracao_media</t>
+  </si>
+  <si>
+    <t>dataMarc</t>
   </si>
 </sst>
 </file>
@@ -1855,10 +1855,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -2251,7 +2251,7 @@
         <v>223</v>
       </c>
       <c r="B1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2335,19 +2335,19 @@
         <v>223</v>
       </c>
       <c r="B1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1" t="s">
         <v>390</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F1" t="s">
         <v>407</v>
-      </c>
-      <c r="D1" t="s">
-        <v>391</v>
-      </c>
-      <c r="E1" t="s">
-        <v>392</v>
-      </c>
-      <c r="F1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18">
@@ -2358,7 +2358,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2386,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2403,7 +2403,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2420,7 +2420,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2459,10 +2459,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2502,13 +2502,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" t="s">
         <v>409</v>
-      </c>
-      <c r="B1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3840,7 +3840,7 @@
         <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C1" t="s">
         <v>361</v>
@@ -4161,7 +4161,7 @@
         <v>383</v>
       </c>
       <c r="C1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4664,8 +4664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF5065-48C3-0D4F-B471-7BBBFE3C553D}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4690,7 +4690,7 @@
         <v>384</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>385</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4853,7 +4853,7 @@
         <v>382</v>
       </c>
       <c r="B1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4861,7 +4861,7 @@
         <v>261</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4869,7 +4869,7 @@
         <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4877,7 +4877,7 @@
         <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4893,7 +4893,7 @@
         <v>295</v>
       </c>
       <c r="B6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4901,7 +4901,7 @@
         <v>295</v>
       </c>
       <c r="B7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4909,7 +4909,7 @@
         <v>300</v>
       </c>
       <c r="B8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4917,7 +4917,7 @@
         <v>303</v>
       </c>
       <c r="B9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4933,7 +4933,7 @@
         <v>318</v>
       </c>
       <c r="B11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4941,7 +4941,7 @@
         <v>333</v>
       </c>
       <c r="B12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4949,7 +4949,7 @@
         <v>338</v>
       </c>
       <c r="B13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -4990,7 +4990,7 @@
         <v>227</v>
       </c>
       <c r="B1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5359,10 +5359,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B1" t="s">
         <v>400</v>
-      </c>
-      <c r="B1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5478,7 +5478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6798383C-D243-9640-A634-7870B6E05811}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -6427,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C1" t="s">
         <v>146</v>
@@ -6436,16 +6436,16 @@
         <v>147</v>
       </c>
       <c r="E1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F1" t="s">
         <v>403</v>
-      </c>
-      <c r="F1" t="s">
-        <v>404</v>
       </c>
       <c r="G1" t="s">
         <v>148</v>
       </c>
       <c r="H1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I1" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
Script done, I guess. Alterações no sp do register para suportar
</commit_message>
<xml_diff>
--- a/Projeto/dados.xlsx
+++ b/Projeto/dados.xlsx
@@ -8,30 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paiva/Documents/Universidade/Engenharia Informática/2º Ano/2º Semestre/Base de Dados/bd/Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1444F083-2606-C146-BDCF-90B869F04953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5873FCF-3ACC-A048-9281-E0E839C7703F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" firstSheet="5" activeTab="8" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
+    <workbookView xWindow="1340" yWindow="-18820" windowWidth="33600" windowHeight="19500" activeTab="4" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
   </bookViews>
   <sheets>
     <sheet name="produto" sheetId="2" r:id="rId1"/>
     <sheet name="promocao" sheetId="4" r:id="rId2"/>
-    <sheet name="cliente" sheetId="10" r:id="rId3"/>
-    <sheet name="cupao" sheetId="3" r:id="rId4"/>
-    <sheet name="contacto" sheetId="7" r:id="rId5"/>
-    <sheet name="utilizador" sheetId="9" r:id="rId6"/>
-    <sheet name="compra" sheetId="8" r:id="rId7"/>
-    <sheet name="servico" sheetId="12" r:id="rId8"/>
-    <sheet name="funcionario" sheetId="11" r:id="rId9"/>
-    <sheet name="cliente_usa_cupao" sheetId="14" r:id="rId10"/>
-    <sheet name="clientefavorita" sheetId="15" r:id="rId11"/>
-    <sheet name="produto_tem_promocao" sheetId="16" r:id="rId12"/>
-    <sheet name="cosmetica" sheetId="5" r:id="rId13"/>
-    <sheet name="perfume" sheetId="6" r:id="rId14"/>
-    <sheet name="compra_presencial" sheetId="19" r:id="rId15"/>
-    <sheet name="compra_online" sheetId="20" r:id="rId16"/>
-    <sheet name="compra_tem_produto" sheetId="17" r:id="rId17"/>
-    <sheet name="funcionario_faz_servico" sheetId="18" r:id="rId18"/>
-    <sheet name="marcacao" sheetId="13" r:id="rId19"/>
+    <sheet name="cupao" sheetId="3" r:id="rId3"/>
+    <sheet name="contacto" sheetId="7" r:id="rId4"/>
+    <sheet name="utilizador" sheetId="9" r:id="rId5"/>
+    <sheet name="compra" sheetId="8" r:id="rId6"/>
+    <sheet name="servico" sheetId="12" r:id="rId7"/>
+    <sheet name="cliente_usa_cupao" sheetId="14" r:id="rId8"/>
+    <sheet name="clientefavorita" sheetId="15" r:id="rId9"/>
+    <sheet name="produto_tem_promocao" sheetId="16" r:id="rId10"/>
+    <sheet name="cosmetica" sheetId="5" r:id="rId11"/>
+    <sheet name="perfume" sheetId="6" r:id="rId12"/>
+    <sheet name="compra_presencial" sheetId="19" r:id="rId13"/>
+    <sheet name="compra_online" sheetId="20" r:id="rId14"/>
+    <sheet name="compra_tem_produto" sheetId="17" r:id="rId15"/>
+    <sheet name="funcionario_faz_servico" sheetId="18" r:id="rId16"/>
+    <sheet name="marcacao" sheetId="13" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="414">
   <si>
     <t>id</t>
   </si>
@@ -2709,308 +2707,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FF32D1-2DB7-7346-9851-10D75E4C5CB3}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>382</v>
-      </c>
-      <c r="B1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="B3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="B4" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B6" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B7" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B8" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B12" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="B13" t="s">
-        <v>388</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{DA82EFA0-17B6-FA41-9F79-DBBDBD19C1DE}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{3D5E5A62-B64A-A547-A880-EF84BDD0FC5A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{19E4FB4E-E475-6240-A5F8-A15995875040}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{FFD81235-1860-954E-81B7-3EE8277262DA}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{0E332F05-B33B-E445-9E47-9B254D4AC342}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{1815BAB9-F47E-1B47-909C-57D98403A338}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{52DA2EAD-018D-264A-9288-37E9CEC837E4}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{0AD9EF88-B92C-5043-AFA7-D082437F18AC}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{7B4B17A5-8D5E-2849-9048-A85057D4D04E}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{8AE7BEDA-C358-9541-A00F-D7DBBDCA68A5}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{A9702B21-31A1-714A-8D38-FC913DD22A85}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{B5F247ED-1128-CB4D-92E1-E2596592F84E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89BB075-E1D3-504E-AEC5-3A48EA5B9950}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B2" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="B4" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B5" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="B7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="B9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="B15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{97DF8CDA-721F-7742-B543-825BC2AB1E07}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{C5C0AA7C-ABE9-C248-84D1-1149C21155F3}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{96389388-1E3D-7C4C-9943-BF4AEEDB39D1}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{F6167ED9-B98D-4B4C-8C78-BA582BEA792F}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{A9284D72-529F-6745-92FA-EBB2BE1E43A4}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{E30E6588-C5AF-DD4D-B0F6-6C849A9B31C6}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{EC3083A8-28DB-A041-87C9-39C2225C2C7D}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{6FC9910C-C0D6-2F44-9D92-16A631888986}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{9E18CD91-06CA-1348-BF63-060C83627FA8}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{B79E2A88-1889-D244-A8E0-4CE39B3072DE}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{E70239DC-2CEE-0E42-B963-1D16AE2150B5}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{B43E3CD7-127D-EF45-AA91-D0A892D7C599}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{A5689E7D-96E8-E742-AA5B-D489DC7981F7}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{1E5FD187-3096-4146-A913-759550C93885}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{1669945E-9C74-D245-A312-4027662EA7A8}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A49931-F752-6145-96A7-CC9432EDD335}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -3141,7 +2837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8FBC05-06AD-494F-BC92-9A5639EAACBF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3188,7 +2884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A585E7F2-9C72-5A49-9138-3F3A64EFA47E}">
   <dimension ref="A1:A23"/>
   <sheetViews>
@@ -3318,7 +3014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D8A57E-9393-F147-92A2-7A71470A8229}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -3400,7 +3096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D32298-08D2-5744-A359-D0D0D1BC1871}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -3572,7 +3268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBABDCBA-3D10-8A4F-BB04-988FC3FBF4BE}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -3821,7 +3517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D9E59B-00B6-9C4C-80BF-EC6AB2822740}">
   <dimension ref="A1:C45"/>
   <sheetViews>
@@ -4342,7 +4038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF5065-48C3-0D4F-B471-7BBBFE3C553D}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -4724,296 +4420,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C5BFFC-CC4E-934C-BDA9-34E72C4908BD}">
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="3">
-        <v>50</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="B4" s="3">
-        <v>100</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="B5" s="3">
-        <v>100</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B7" s="3">
-        <v>200</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B8" s="3">
-        <v>150</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="B9" s="3">
-        <v>50</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10" s="3">
-        <v>100</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B12" s="3">
-        <v>250</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B15" s="3">
-        <v>50</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="B16" s="3">
-        <v>100</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E900CA9A-64A6-0F41-A83E-BF1433A95A1A}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{79E8E305-74F0-FF46-B6F4-3CEFF7C34F06}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{D4FE4473-072F-F14A-A5F9-2D6F7848A73E}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{C184E322-E316-754B-AB6B-8D7DF9B76B65}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{5C898094-8851-6A4C-A653-AFD6A64F3ED4}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{5D5ED531-8D4A-1E44-A1F8-815D0405A45C}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{9434A901-4E77-D24C-9005-CD295F8A130A}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{509769C7-4E41-4045-B6DD-9A908DBC4526}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{E2E55D28-47A1-FA42-B446-CAD1EC6C3005}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{ED6C6564-E4C1-0646-860F-145DA6319402}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{17E78FF8-9921-504F-AC3D-A6FB98DC240E}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{49DA98EF-68FE-F24F-9D2E-D66BD1913A9A}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{69C23839-16F8-A84E-B190-0BFFC7B06082}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{8E12BCEA-E2CA-114F-8D24-CE493DA93847}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{89E3D340-F514-BC42-9C6C-F1D0E49F77D2}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{CCA00291-60C1-2F4B-9659-96DF991E537C}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{D02EF134-B1A8-0748-B3D9-CDAD47A7B360}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECE3593-E1CC-8E4B-A47B-B25F5CCC3F7D}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -5200,7 +4606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9452136D-12A1-A84C-959A-D16ED4D29668}">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -5841,13 +5247,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF85F82-A4D9-A940-ADAE-CD03F7BD19F3}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -5858,9 +5262,10 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
         <v>248</v>
       </c>
@@ -5888,8 +5293,23 @@
       <c r="I1" s="3" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="M1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>256</v>
       </c>
@@ -5917,8 +5337,14 @@
       <c r="I2" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>261</v>
       </c>
@@ -5946,8 +5372,17 @@
       <c r="I3" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="3">
+        <v>50</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>267</v>
       </c>
@@ -5975,8 +5410,14 @@
       <c r="I4" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>272</v>
       </c>
@@ -6004,8 +5445,17 @@
       <c r="I5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="4" t="s">
         <v>277</v>
       </c>
@@ -6033,8 +5483,17 @@
       <c r="I6" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="3">
+        <v>100</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="4" t="s">
         <v>282</v>
       </c>
@@ -6062,8 +5521,17 @@
       <c r="I7" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="3">
+        <v>100</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
         <v>286</v>
       </c>
@@ -6091,8 +5559,17 @@
       <c r="I8" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
         <v>291</v>
       </c>
@@ -6120,8 +5597,17 @@
       <c r="I9" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="3">
+        <v>200</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
         <v>295</v>
       </c>
@@ -6149,8 +5635,17 @@
       <c r="I10" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="3">
+        <v>150</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
         <v>300</v>
       </c>
@@ -6178,8 +5673,17 @@
       <c r="I11" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="3">
+        <v>50</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="7" t="s">
         <v>303</v>
       </c>
@@ -6207,8 +5711,17 @@
       <c r="I12" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="3">
+        <v>100</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="7" t="s">
         <v>308</v>
       </c>
@@ -6236,8 +5749,17 @@
       <c r="I13" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="7" t="s">
         <v>313</v>
       </c>
@@ -6265,8 +5787,14 @@
       <c r="I14" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="7" t="s">
         <v>318</v>
       </c>
@@ -6294,8 +5822,17 @@
       <c r="I15" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="3">
+        <v>250</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
         <v>323</v>
       </c>
@@ -6323,8 +5860,17 @@
       <c r="I16" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="7" t="s">
         <v>328</v>
       </c>
@@ -6352,8 +5898,17 @@
       <c r="I17" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="7" t="s">
         <v>333</v>
       </c>
@@ -6381,8 +5936,17 @@
       <c r="I18" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="3">
+        <v>50</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="7" t="s">
         <v>338</v>
       </c>
@@ -6410,8 +5974,17 @@
       <c r="I19" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="3">
+        <v>100</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="7" t="s">
         <v>343</v>
       </c>
@@ -6439,8 +6012,17 @@
       <c r="I20" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="7" t="s">
         <v>348</v>
       </c>
@@ -6468,8 +6050,17 @@
       <c r="I21" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="7" t="s">
         <v>353</v>
       </c>
@@ -6497,8 +6088,14 @@
       <c r="I22" s="6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6509,7 +6106,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:14">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6520,7 +6117,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:14">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6531,7 +6128,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:14">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6542,7 +6139,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:14">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6553,7 +6150,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:14">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6564,7 +6161,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:14">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6575,7 +6172,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:14">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6635,7 +6232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A7E83F-E041-C842-8279-D6424662D499}">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -6982,7 +6579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3F6A38-D1AE-A74B-BE47-CADD5261F43E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -7220,82 +6817,303 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB199FB-4085-7A4D-933D-5B11F2AC9371}">
-  <dimension ref="A1:C5"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FF32D1-2DB7-7346-9851-10D75E4C5CB3}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>261</v>
+      </c>
+      <c r="B2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>750</v>
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B13" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{5EA6DBC4-23B6-1640-B636-F3A85D57D019}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6501B208-EE99-A347-90F7-E0B6314A844C}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{9108A297-E545-B94C-9C34-0031DFFF5A24}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{85B2F76B-25AE-874E-860B-8B26FFC57A7C}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DA82EFA0-17B6-FA41-9F79-DBBDBD19C1DE}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3D5E5A62-B64A-A547-A880-EF84BDD0FC5A}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{19E4FB4E-E475-6240-A5F8-A15995875040}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{FFD81235-1860-954E-81B7-3EE8277262DA}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{0E332F05-B33B-E445-9E47-9B254D4AC342}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{1815BAB9-F47E-1B47-909C-57D98403A338}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{52DA2EAD-018D-264A-9288-37E9CEC837E4}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{0AD9EF88-B92C-5043-AFA7-D082437F18AC}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{7B4B17A5-8D5E-2849-9048-A85057D4D04E}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{8AE7BEDA-C358-9541-A00F-D7DBBDCA68A5}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{A9702B21-31A1-714A-8D38-FC913DD22A85}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{B5F247ED-1128-CB4D-92E1-E2596592F84E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89BB075-E1D3-504E-AEC5-3A48EA5B9950}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{97DF8CDA-721F-7742-B543-825BC2AB1E07}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C5C0AA7C-ABE9-C248-84D1-1149C21155F3}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{96389388-1E3D-7C4C-9943-BF4AEEDB39D1}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{F6167ED9-B98D-4B4C-8C78-BA582BEA792F}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{A9284D72-529F-6745-92FA-EBB2BE1E43A4}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{E30E6588-C5AF-DD4D-B0F6-6C849A9B31C6}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{EC3083A8-28DB-A041-87C9-39C2225C2C7D}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{6FC9910C-C0D6-2F44-9D92-16A631888986}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{9E18CD91-06CA-1348-BF63-060C83627FA8}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{B79E2A88-1889-D244-A8E0-4CE39B3072DE}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{E70239DC-2CEE-0E42-B963-1D16AE2150B5}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{B43E3CD7-127D-EF45-AA91-D0A892D7C599}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{A5689E7D-96E8-E742-AA5B-D489DC7981F7}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{1E5FD187-3096-4146-A913-759550C93885}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{1669945E-9C74-D245-A312-4027662EA7A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Script de inserção e itnerface
</commit_message>
<xml_diff>
--- a/Projeto/dados.xlsx
+++ b/Projeto/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paiva/Documents/Universidade/Engenharia Informática/2º Ano/2º Semestre/Base de Dados/bd/Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5873FCF-3ACC-A048-9281-E0E839C7703F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E041C7-BD3A-2642-88C0-228328489335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="-18820" windowWidth="33600" windowHeight="19500" activeTab="4" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="33600" windowHeight="19500" activeTab="3" xr2:uid="{2AE14976-DDCE-6441-9BEC-2FCE017ACED9}"/>
   </bookViews>
   <sheets>
     <sheet name="produto" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="415">
   <si>
     <t>id</t>
   </si>
@@ -279,18 +279,12 @@
     <t>Azzaro Pour Homme</t>
   </si>
   <si>
-    <t>Azzaro Pour Homme é um perfume de sedução em estado puro, talhado pela elegância e pelo requinte italiano. Com esta versão Intense, a fragrância torna-se mais sofisticada e mais intensa, para homens que apreciam a nobreza das belas matérias. A fragrância foi construída em Azzaro Pour Homme é um perfume de sedução em estado puro, talhado pela elegância e pelo requinte italiano. Com esta versão Intense, a fragrância torna-se mais sofisticada e mais intensa, para homens que apreciam a nobreza das belas matérias. A fragrância foi construída em torno de um acorde único de canela, vétiver e fava tonka.</t>
-  </si>
-  <si>
     <t>https://www.perfumesecompanhia.pt/fotos/produtos/3351500980543_1.jpg</t>
   </si>
   <si>
     <t>Deo Spray</t>
   </si>
   <si>
-    <t>Num gesto só, este spray oferece uma proteção eficaz de longa duração e uma sensação de frescura, durante todo o dia. É muito suave, à base de álcool mas a sua fórmula não irritante oferece resultados de ação tripla: desodorizante, regulador e calmante. Com um toque final refinado, que deixa a pele subtilmente perfumada com as notas irresistíveis de Azzaro Pour Homme.</t>
-  </si>
-  <si>
     <t>https://www.perfumesecompanhia.pt/fotos/produtos/3351500002771_1.jpg</t>
   </si>
   <si>
@@ -333,9 +327,6 @@
     <t>Azzaro Chrome</t>
   </si>
   <si>
-    <t>A assinatura emblemática de Chrome —um acorde cítrico e amadeirado, ao qual se acrescenta um grande coração aquático, que inspira frescura e força — é reinterpretada numa fórmula original 100% sem álcool, substituído pela água. A frescura imiscui-se por toda a parte, sendo ainda mais extrema. Desde a aplicação, uma sensação revigorante impregna-se na pele. Esta frescura instantânea manifesta um efeito gélido imediato, como uma frescura polar.</t>
-  </si>
-  <si>
     <t>https://www.perfumesecompanhia.pt/fotos/produtos/3351500009756_1.jpg</t>
   </si>
   <si>
@@ -396,9 +387,6 @@
     <t>https://www.perfumesecompanhia.pt/fotos/produtos/0022548055373.jpg</t>
   </si>
   <si>
-    <t>Anti-Perspirant Deodorant Stick</t>
-  </si>
-  <si>
     <t>https://www.perfumesecompanhia.pt/fotos/produtos/0022548024355_1.jpg</t>
   </si>
   <si>
@@ -462,9 +450,6 @@
     <t>Tónico de Banho</t>
   </si>
   <si>
-    <t>Para transformar cada cm² da sua pele e a tornar mais lisa e bela - mais tonificada, mais fina e maravilhosamente nutrida. Este cuidado de limpeza concentrado activa-se sob o efeito do calor do banho ou do duche - libertando os seus vapores aromáticos tonificantes de Alecrim, Hortelã e Gerânio.</t>
-  </si>
-  <si>
     <t>https://www.perfumesecompanhia.pt/fotos/produtos/3380810667103.jpg</t>
   </si>
   <si>
@@ -522,9 +507,6 @@
     <t>Avenida 5 de Outubro</t>
   </si>
   <si>
-    <t>Nº 9</t>
-  </si>
-  <si>
     <t>4750-765</t>
   </si>
   <si>
@@ -543,9 +525,6 @@
     <t>Rua dos Azinhais</t>
   </si>
   <si>
-    <t>Nº 6</t>
-  </si>
-  <si>
     <t>Esporões</t>
   </si>
   <si>
@@ -570,9 +549,6 @@
     <t>Rua Olival de Cambra</t>
   </si>
   <si>
-    <t>Urbanização Casal do Rebentão Nº2, 3º Esquerdo</t>
-  </si>
-  <si>
     <t>4420-133</t>
   </si>
   <si>
@@ -1291,6 +1267,33 @@
   </si>
   <si>
     <t>deleted</t>
+  </si>
+  <si>
+    <t>Azzaro Pour Homme é um perfume de sedução em estado puro, talhado pela elegância e pelo requinte italiano.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num gesto só, este spray oferece uma proteção eficaz de longa duração e uma sensação de frescura, durante todo o dia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A assinatura emblemática de Chrome —um acorde cítrico e amadeirado, ao qual se acrescenta um grande coração aquático, que inspira frescura e força — é reinterpretada numa fórmula original 100% sem álcool, substituído pela água. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para transformar cada cm² da sua pele e a tornar mais lisa e bela - mais tonificada, mais fina e maravilhosamente nutrida. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-Perspirant Deodorant </t>
+  </si>
+  <si>
+    <t>Nº2, 3º Esquerdo</t>
+  </si>
+  <si>
+    <t>Nº9</t>
+  </si>
+  <si>
+    <t>Nº5</t>
+  </si>
+  <si>
+    <t>Nº6</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1392,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1406,7 +1409,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1704,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6798383C-D243-9640-A634-7870B6E05811}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1717,8 +1720,8 @@
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" customWidth="1"/>
+    <col min="10" max="10" width="157.1640625" customWidth="1"/>
     <col min="11" max="11" width="22.83203125" customWidth="1"/>
     <col min="12" max="12" width="25.5" customWidth="1"/>
   </cols>
@@ -1728,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -1761,7 +1764,7 @@
         <v>67</v>
       </c>
       <c r="M1" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1775,10 +1778,10 @@
         <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
         <v>70</v>
@@ -1816,10 +1819,10 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
         <v>70</v>
@@ -1857,10 +1860,10 @@
         <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
         <v>70</v>
@@ -1872,10 +1875,10 @@
         <v>100</v>
       </c>
       <c r="I4" t="s">
+        <v>406</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1895,10 +1898,10 @@
         <v>27.2</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
         <v>70</v>
@@ -1910,10 +1913,10 @@
         <v>150</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>407</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -1933,31 +1936,31 @@
         <v>77.3</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H6">
         <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K6">
         <v>10</v>
       </c>
       <c r="L6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1971,25 +1974,25 @@
         <v>75.25</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7" t="s">
         <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7" t="s">
-        <v>94</v>
+        <v>408</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -2009,28 +2012,28 @@
         <v>78.709999999999994</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H8">
         <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -2050,28 +2053,28 @@
         <v>104.95</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K9">
         <v>4</v>
@@ -2091,28 +2094,28 @@
         <v>140.65</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H10">
         <v>200</v>
       </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K10">
         <v>5</v>
@@ -2132,28 +2135,28 @@
         <v>27.3</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H11">
         <v>75</v>
       </c>
       <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="K11">
         <v>6</v>
@@ -2173,28 +2176,28 @@
         <v>27.3</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H12">
         <v>150</v>
       </c>
       <c r="I12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K12">
         <v>7</v>
@@ -2214,28 +2217,28 @@
         <v>72.5</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H13">
         <v>50</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K13">
         <v>2</v>
       </c>
       <c r="L13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2249,28 +2252,28 @@
         <v>47.5</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H14">
         <v>200</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K14">
         <v>5</v>
       </c>
       <c r="L14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2284,19 +2287,19 @@
         <v>77.900000000000006</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K15">
         <v>5</v>
@@ -2316,22 +2319,22 @@
         <v>22.28</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H16">
         <v>30</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K16">
         <v>2</v>
@@ -2351,22 +2354,22 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H17">
         <v>50</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K17">
         <v>3</v>
@@ -2386,22 +2389,22 @@
         <v>50.2</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H18">
         <v>100</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K18">
         <v>4</v>
@@ -2421,22 +2424,22 @@
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>410</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H19">
         <v>75</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K19">
         <v>2</v>
@@ -2456,25 +2459,25 @@
         <v>29.7</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H20">
         <v>30</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -2488,25 +2491,25 @@
         <v>39.950000000000003</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H21">
         <v>50</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K21">
         <v>6</v>
       </c>
       <c r="L21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -2520,28 +2523,28 @@
         <v>47.45</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H22">
         <v>100</v>
       </c>
       <c r="I22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -2555,31 +2558,31 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H23">
         <v>100</v>
       </c>
       <c r="I23" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K23">
         <v>5</v>
       </c>
       <c r="L23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -2593,19 +2596,19 @@
         <v>38.65</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H24">
         <v>125</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K24">
         <v>6</v>
@@ -2622,22 +2625,22 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H25">
         <v>200</v>
       </c>
       <c r="I25" t="s">
-        <v>137</v>
+        <v>409</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2654,19 +2657,19 @@
         <v>32.950000000000003</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F26" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H26">
         <v>100</v>
       </c>
       <c r="J26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K26">
         <v>3</v>
@@ -2722,10 +2725,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2852,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2860,7 +2863,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2868,7 +2871,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2876,7 +2879,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3029,10 +3032,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3040,7 +3043,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3048,7 +3051,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3056,7 +3059,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3064,7 +3067,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3072,7 +3075,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3080,7 +3083,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3113,22 +3116,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C1" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="D1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="E1" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="F1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18">
@@ -3139,7 +3142,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3167,7 +3170,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3184,7 +3187,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3201,7 +3204,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -3240,10 +3243,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3283,13 +3286,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C1" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3533,18 +3536,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B1" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3555,7 +3558,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3566,7 +3569,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3577,7 +3580,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -3588,7 +3591,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -3599,7 +3602,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -3610,7 +3613,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -3621,7 +3624,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B9">
         <v>19</v>
@@ -3632,7 +3635,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3643,7 +3646,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -3654,7 +3657,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -3665,7 +3668,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -3676,7 +3679,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -3687,7 +3690,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -3698,7 +3701,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -3709,7 +3712,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B17">
         <v>13</v>
@@ -3720,7 +3723,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -3731,7 +3734,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -3742,7 +3745,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -3753,7 +3756,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B21">
         <v>14</v>
@@ -3764,7 +3767,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B22">
         <v>16</v>
@@ -3775,7 +3778,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B23">
         <v>17</v>
@@ -3786,7 +3789,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B24">
         <v>18</v>
@@ -3797,7 +3800,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B25">
         <v>19</v>
@@ -3808,7 +3811,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3819,7 +3822,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -3830,7 +3833,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -3841,7 +3844,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -3852,7 +3855,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -3863,7 +3866,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -3874,7 +3877,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B32">
         <v>7</v>
@@ -3885,7 +3888,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3896,7 +3899,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B34">
         <v>9</v>
@@ -3907,7 +3910,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B35">
         <v>10</v>
@@ -3918,7 +3921,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B36">
         <v>11</v>
@@ -3929,7 +3932,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B37">
         <v>12</v>
@@ -3940,7 +3943,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B38">
         <v>13</v>
@@ -3951,7 +3954,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B39">
         <v>14</v>
@@ -3962,7 +3965,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B40">
         <v>15</v>
@@ -3973,7 +3976,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B41">
         <v>16</v>
@@ -3984,7 +3987,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B42">
         <v>17</v>
@@ -3995,7 +3998,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B43">
         <v>18</v>
@@ -4006,7 +4009,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B44">
         <v>19</v>
@@ -4059,16 +4062,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4076,13 +4079,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E2" s="10">
         <v>43966.6875</v>
@@ -4093,13 +4096,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C3" s="1">
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E3" s="10">
         <v>43996.395833333336</v>
@@ -4110,13 +4113,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C4" s="1">
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E4" s="10">
         <v>43962.791666666664</v>
@@ -4127,13 +4130,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="E5" s="10">
         <v>43985.625</v>
@@ -4144,13 +4147,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C6" s="1">
         <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E6" s="10">
         <v>44014.479166666664</v>
@@ -4161,13 +4164,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E7" s="10">
         <v>43966.729166666664</v>
@@ -4178,13 +4181,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C8" s="1">
         <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E8" s="10">
         <v>43974.59375</v>
@@ -4575,10 +4578,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B11" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -4589,10 +4592,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B12" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -4610,8 +4613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9452136D-12A1-A84C-959A-D16ED4D29668}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4621,8 +4624,8 @@
     <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="7" max="7" width="76.5" customWidth="1"/>
+    <col min="8" max="8" width="49" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4631,28 +4634,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E1" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="F1" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H1" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="I1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4660,7 +4663,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C2">
         <v>914363252</v>
@@ -4669,16 +4672,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4686,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C3">
         <v>924763965</v>
@@ -4695,19 +4698,19 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" t="s">
         <v>151</v>
       </c>
-      <c r="G3" t="s">
-        <v>156</v>
-      </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>412</v>
       </c>
       <c r="I3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4715,7 +4718,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C4">
         <v>914274915</v>
@@ -4724,19 +4727,19 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>413</v>
       </c>
       <c r="I4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4744,7 +4747,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C5">
         <v>964829602</v>
@@ -4753,19 +4756,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H5" t="s">
-        <v>164</v>
+        <v>414</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4773,7 +4776,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C6">
         <v>935502152</v>
@@ -4782,19 +4785,19 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H6" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4802,7 +4805,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C7">
         <v>914628560</v>
@@ -4811,19 +4814,19 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G7" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H7" t="s">
-        <v>173</v>
+        <v>411</v>
       </c>
       <c r="I7" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4831,7 +4834,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C8">
         <v>963926453</v>
@@ -4840,19 +4843,19 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G8" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H8" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4860,7 +4863,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C9">
         <v>921547935</v>
@@ -4869,19 +4872,19 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I9" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4889,7 +4892,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C10">
         <v>918426539</v>
@@ -4898,19 +4901,19 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G10" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="I10" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4918,7 +4921,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C11">
         <v>963159731</v>
@@ -4927,19 +4930,19 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F11" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G11" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H11" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I11" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4947,7 +4950,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C12">
         <v>936267422</v>
@@ -4956,16 +4959,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G12" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I12" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4973,7 +4976,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C13">
         <v>926375015</v>
@@ -4982,19 +4985,19 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G13" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H13" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I13" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -5002,7 +5005,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C14">
         <v>963216832</v>
@@ -5011,19 +5014,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G14" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H14" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -5031,7 +5034,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C15">
         <v>915392054</v>
@@ -5040,16 +5043,16 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G15" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -5057,7 +5060,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C16">
         <v>964667921</v>
@@ -5066,19 +5069,19 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G16" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H16" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I16" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -5086,7 +5089,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C17">
         <v>962468333</v>
@@ -5095,19 +5098,19 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G17" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H17" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I17" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -5115,7 +5118,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C18">
         <v>925488312</v>
@@ -5124,19 +5127,19 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F18" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G18" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H18" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="I18" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -5144,7 +5147,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C19">
         <v>915424675</v>
@@ -5153,16 +5156,16 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I19" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -5170,7 +5173,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C20">
         <v>963215352</v>
@@ -5179,19 +5182,19 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F20" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G20" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H20" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="I20" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -5199,7 +5202,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C21">
         <v>924583100</v>
@@ -5208,16 +5211,16 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G21" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="I21" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5251,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF85F82-A4D9-A940-ADAE-CD03F7BD19F3}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -5267,63 +5270,63 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="M1" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="N1" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B2" s="3">
         <v>287567665</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -5332,7 +5335,7 @@
         <v>31905</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="I2" s="3">
         <v>2</v>
@@ -5346,19 +5349,19 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3">
         <v>457253189</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -5367,10 +5370,10 @@
         <v>34368</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J3" s="3">
         <v>50</v>
@@ -5379,24 +5382,24 @@
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B4" s="3">
         <v>998232166</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -5405,10 +5408,10 @@
         <v>37279</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -5419,19 +5422,19 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B5" s="3">
         <v>397543100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5440,7 +5443,7 @@
         <v>36135</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
@@ -5452,24 +5455,24 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B6" s="3">
         <v>302167890</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -5478,10 +5481,10 @@
         <v>22224</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J6" s="3">
         <v>100</v>
@@ -5490,24 +5493,24 @@
         <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B7" s="3">
         <v>592165320</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -5516,10 +5519,10 @@
         <v>34956</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J7" s="3">
         <v>100</v>
@@ -5528,24 +5531,24 @@
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B8" s="3">
         <v>943212111</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -5554,7 +5557,7 @@
         <v>36292</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="I8" s="3">
         <v>14</v>
@@ -5566,24 +5569,24 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B9" s="3">
         <v>123222985</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -5592,10 +5595,10 @@
         <v>38708</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J9" s="3">
         <v>200</v>
@@ -5604,24 +5607,24 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B10" s="3">
         <v>445976504</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -5630,10 +5633,10 @@
         <v>33061</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J10" s="3">
         <v>150</v>
@@ -5642,24 +5645,24 @@
         <v>1</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B11" s="3">
         <v>455129988</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -5668,7 +5671,7 @@
         <v>36651</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="I11" s="3">
         <v>4</v>
@@ -5680,24 +5683,24 @@
         <v>0</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="7" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B12" s="3">
         <v>178495829</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -5706,10 +5709,10 @@
         <v>38266</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J12" s="3">
         <v>100</v>
@@ -5718,24 +5721,24 @@
         <v>0</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="7" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B13" s="3">
         <v>125873530</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -5744,7 +5747,7 @@
         <v>26474</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I13" s="3">
         <v>8</v>
@@ -5756,24 +5759,24 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="7" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B14" s="3">
         <v>573975939</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="F14" s="3">
         <v>0</v>
@@ -5782,10 +5785,10 @@
         <v>36199</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -5796,19 +5799,19 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B15" s="3">
         <v>258759872</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -5817,7 +5820,7 @@
         <v>31077</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="I15" s="3">
         <v>9</v>
@@ -5829,24 +5832,24 @@
         <v>0</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B16" s="3">
         <v>287352385</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
@@ -5855,7 +5858,7 @@
         <v>36647</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="I16" s="3">
         <v>10</v>
@@ -5867,24 +5870,24 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="7" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B17" s="3">
         <v>821358756</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -5893,10 +5896,10 @@
         <v>32766</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J17" s="3">
         <v>0</v>
@@ -5905,24 +5908,24 @@
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="7" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B18" s="3">
         <v>602941753</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -5931,7 +5934,7 @@
         <v>37289</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="I18" s="3">
         <v>11</v>
@@ -5943,24 +5946,24 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="7" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B19" s="3">
         <v>219589974</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -5969,10 +5972,10 @@
         <v>24101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J19" s="3">
         <v>100</v>
@@ -5981,24 +5984,24 @@
         <v>1</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="7" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B20" s="3">
         <v>476638927</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
@@ -6007,10 +6010,10 @@
         <v>35868</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="J20" s="3">
         <v>0</v>
@@ -6019,24 +6022,24 @@
         <v>1</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="7" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B21" s="3">
         <v>593967351</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -6045,7 +6048,7 @@
         <v>29006</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="I21" s="3">
         <v>12</v>
@@ -6057,24 +6060,24 @@
         <v>1</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B22" s="3">
         <v>129885782</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F22" s="3">
         <v>0</v>
@@ -6083,10 +6086,10 @@
         <v>25857</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -6252,25 +6255,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="G1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6284,7 +6287,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -6301,10 +6304,10 @@
         <v>37121343</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6321,10 +6324,10 @@
         <v>60474094</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -6341,10 +6344,10 @@
         <v>86134119</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -6361,10 +6364,10 @@
         <v>6421976</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D6" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -6381,10 +6384,10 @@
         <v>299678786</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -6401,10 +6404,10 @@
         <v>111498402</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -6421,10 +6424,10 @@
         <v>108025260</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D9" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -6441,10 +6444,10 @@
         <v>141414204</v>
       </c>
       <c r="C10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D10" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -6461,10 +6464,10 @@
         <v>56737679</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D11" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -6481,10 +6484,10 @@
         <v>3544357</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -6501,10 +6504,10 @@
         <v>196674321</v>
       </c>
       <c r="C13" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -6521,10 +6524,10 @@
         <v>196954062</v>
       </c>
       <c r="C14" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -6541,10 +6544,10 @@
         <v>42896574</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F15">
         <v>20</v>
@@ -6561,10 +6564,10 @@
         <v>112964237</v>
       </c>
       <c r="C16" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D16" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -6597,10 +6600,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -6608,7 +6611,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C2">
         <v>45.5</v>
@@ -6619,7 +6622,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C3">
         <v>7.5</v>
@@ -6630,7 +6633,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C4">
         <v>12.8</v>
@@ -6641,7 +6644,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C5">
         <v>9.5</v>
@@ -6652,7 +6655,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -6663,7 +6666,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -6674,7 +6677,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C8">
         <v>85</v>
@@ -6685,7 +6688,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C9">
         <v>35.700000000000003</v>
@@ -6696,7 +6699,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C10">
         <v>24.5</v>
@@ -6707,7 +6710,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C11">
         <v>47</v>
@@ -6718,7 +6721,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C12">
         <v>14.99</v>
@@ -6729,7 +6732,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C13">
         <v>17.899999999999999</v>
@@ -6740,7 +6743,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -6751,7 +6754,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C15">
         <v>19.989999999999998</v>
@@ -6762,7 +6765,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C16">
         <v>25.15</v>
@@ -6773,7 +6776,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C17">
         <v>23</v>
@@ -6784,7 +6787,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C18">
         <v>67.900000000000006</v>
@@ -6795,7 +6798,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C19">
         <v>20.149999999999999</v>
@@ -6806,7 +6809,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C20">
         <v>71</v>
@@ -6834,39 +6837,39 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B1" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -6874,39 +6877,39 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B6" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B8" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B9" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -6914,26 +6917,26 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B11" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B12" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="7" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -6971,15 +6974,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
@@ -6987,7 +6990,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -6995,7 +6998,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B4" s="1">
         <v>6</v>
@@ -7003,7 +7006,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
@@ -7011,7 +7014,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -7019,7 +7022,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B7">
         <v>13</v>
@@ -7027,7 +7030,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -7035,7 +7038,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -7043,7 +7046,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -7051,7 +7054,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -7059,7 +7062,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -7067,7 +7070,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="7" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -7075,7 +7078,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B14">
         <v>16</v>
@@ -7083,7 +7086,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -7091,7 +7094,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="4" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B16">
         <v>20</v>

</xml_diff>